<commit_message>
feat: update data loading logic and enhance database schema for trade confirmations
</commit_message>
<xml_diff>
--- a/utility/WSS_Data.xlsx
+++ b/utility/WSS_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>currency</t>
   </si>
@@ -27,21 +27,9 @@
     <t>settlement_amount</t>
   </si>
   <si>
-    <t>nominal_amount_or_quantity</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
     <t>isin</t>
   </si>
   <si>
-    <t>value_or_settlement_date</t>
-  </si>
-  <si>
-    <t>standard_settlement_instruction</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -54,23 +42,72 @@
     <t>US6937512345</t>
   </si>
   <si>
-    <t>Delivery Versus Payment By UB Agent: Stream A/c 19200 Our Beneficiary Swift Code BKBKBK32 Our Agent BIC Code BKBKBKBK</t>
-  </si>
-  <si>
     <t>US9127123213</t>
   </si>
   <si>
     <t>PSET FFFF33</t>
   </si>
   <si>
-    <t>date_of_creation</t>
+    <t>buy_sell</t>
+  </si>
+  <si>
+    <t>settlement_date</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>creation_date</t>
+  </si>
+  <si>
+    <t>Stream A/c 19200 Our Beneficiary Swift Code BKBKBK32 Our Agent BIC Code BKBKBKBK</t>
+  </si>
+  <si>
+    <t>Our Settlement Instructions BANK OF NEW YORK, NEW YORK (BDS) FXF  Your Settlement Instructions CITBNK N.A. 0854CS104</t>
+  </si>
+  <si>
+    <t>US912812313</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOLDMAN SACHS
+/ER/1111
+CLIENT
+/ER/2222
+</t>
+  </si>
+  <si>
+    <t>FR00123123</t>
+  </si>
+  <si>
+    <t>US9127111117</t>
+  </si>
+  <si>
+    <t>0213123131089 CINK NYC
+CUST
+A/C 11111
+XXX12323
+Our Settlement:
+ABA # 03123123118 BK OF NYC/1231313, CIOUP GLOBAL MARKETS INC AS SETTLEMENT AGENT FOR 1231</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +133,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,27 +427,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -411,71 +455,128 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45252</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>11948200</v>
-      </c>
-      <c r="D2">
-        <v>12000000</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11849200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
         <v>45983</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45220</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>19777430.559999999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>19777430.559999999</v>
-      </c>
-      <c r="D3">
-        <v>20000000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3" s="1">
         <v>45951</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29851455.460000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45931</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12312960</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45932</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45978</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>33862165.869999997</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45978</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>